<commit_message>
update the metacoder visualization ananlysis
</commit_message>
<xml_diff>
--- a/step2_kraken2_analysis/unique_genera.xlsx
+++ b/step2_kraken2_analysis/unique_genera.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcmedu-my.sharepoint.com/personal/jochum_bcm_edu/Documents/Documents/github/microbial/step2_kraken2_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{E7625182-F1DE-456A-9A94-11962FF4C571}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E0B6CAE7-BF60-43C0-8DD9-147354747F59}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{E7625182-F1DE-456A-9A94-11962FF4C571}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{827FF0C6-0D12-4CB9-84FE-9575E80183B9}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="600" windowWidth="21390" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unique_genera" sheetId="1" r:id="rId1"/>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,22 +1066,22 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
       <c r="J2">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K2">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L2">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M2">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1107,22 +1107,22 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
       <c r="J3">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K3">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L3">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M3">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1148,22 +1148,22 @@
         <v>22</v>
       </c>
       <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
         <v>37</v>
       </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
       <c r="J4">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K4">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L4">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M4">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1189,22 +1189,22 @@
         <v>28</v>
       </c>
       <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
         <v>37</v>
       </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
       <c r="J5">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K5">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L5">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M5">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1230,22 +1230,22 @@
         <v>23</v>
       </c>
       <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
         <v>37</v>
       </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
       <c r="J6">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K6">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L6">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M6">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1271,22 +1271,22 @@
         <v>27</v>
       </c>
       <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
         <v>37</v>
       </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
       <c r="J7">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K7">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L7">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M7">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1312,22 +1312,22 @@
         <v>36</v>
       </c>
       <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
         <v>37</v>
       </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
       <c r="J8">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K8">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L8">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M8">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1353,22 +1353,22 @@
         <v>33</v>
       </c>
       <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
         <v>37</v>
       </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
       <c r="J9">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K9">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L9">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M9">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1394,22 +1394,22 @@
         <v>25</v>
       </c>
       <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
         <v>37</v>
       </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
       <c r="J10">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K10">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L10">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M10">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1435,22 +1435,22 @@
         <v>31</v>
       </c>
       <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
         <v>37</v>
       </c>
-      <c r="I11" t="s">
-        <v>18</v>
-      </c>
       <c r="J11">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K11">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L11">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M11">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1476,22 +1476,22 @@
         <v>29</v>
       </c>
       <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
         <v>37</v>
       </c>
-      <c r="I12" t="s">
-        <v>18</v>
-      </c>
       <c r="J12">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K12">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L12">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M12">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1517,22 +1517,22 @@
         <v>26</v>
       </c>
       <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
         <v>37</v>
       </c>
-      <c r="I13" t="s">
-        <v>18</v>
-      </c>
       <c r="J13">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K13">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L13">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M13">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1558,22 +1558,22 @@
         <v>30</v>
       </c>
       <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
         <v>37</v>
       </c>
-      <c r="I14" t="s">
-        <v>18</v>
-      </c>
       <c r="J14">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K14">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L14">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M14">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1599,22 +1599,22 @@
         <v>35</v>
       </c>
       <c r="H15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" t="s">
         <v>37</v>
       </c>
-      <c r="I15" t="s">
-        <v>18</v>
-      </c>
       <c r="J15">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K15">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L15">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M15">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1640,22 +1640,22 @@
         <v>24</v>
       </c>
       <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
         <v>37</v>
       </c>
-      <c r="I16" t="s">
-        <v>18</v>
-      </c>
       <c r="J16">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K16">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L16">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M16">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1681,22 +1681,22 @@
         <v>34</v>
       </c>
       <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" t="s">
         <v>37</v>
       </c>
-      <c r="I17" t="s">
-        <v>18</v>
-      </c>
       <c r="J17">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K17">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L17">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M17">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1722,22 +1722,22 @@
         <v>32</v>
       </c>
       <c r="H18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
         <v>37</v>
       </c>
-      <c r="I18" t="s">
-        <v>18</v>
-      </c>
       <c r="J18">
-        <v>2.3290013895483099</v>
+        <v>-4.3828801732468596</v>
       </c>
       <c r="K18">
-        <v>-7.27945437385248E-2</v>
+        <v>-0.458701859982933</v>
       </c>
       <c r="L18">
-        <v>-0.13322808293229399</v>
-      </c>
-      <c r="M18">
-        <v>6.7236393232537103E-3</v>
+        <v>-0.37665062790661402</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1.6856176183356099E-8</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1763,22 +1763,22 @@
         <v>16</v>
       </c>
       <c r="H19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" t="s">
         <v>37</v>
       </c>
-      <c r="I19" t="s">
-        <v>18</v>
-      </c>
       <c r="J19">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K19" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K19">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L19">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M19">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1804,22 +1804,22 @@
         <v>16</v>
       </c>
       <c r="H20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" t="s">
         <v>37</v>
       </c>
-      <c r="I20" t="s">
-        <v>18</v>
-      </c>
       <c r="J20">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K20" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K20">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L20">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M20">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1845,22 +1845,22 @@
         <v>22</v>
       </c>
       <c r="H21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" t="s">
         <v>37</v>
       </c>
-      <c r="I21" t="s">
-        <v>18</v>
-      </c>
       <c r="J21">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K21" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K21">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L21">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M21">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1886,22 +1886,22 @@
         <v>28</v>
       </c>
       <c r="H22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
         <v>37</v>
       </c>
-      <c r="I22" t="s">
-        <v>18</v>
-      </c>
       <c r="J22">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K22" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K22">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L22">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M22">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1927,22 +1927,22 @@
         <v>23</v>
       </c>
       <c r="H23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" t="s">
         <v>37</v>
       </c>
-      <c r="I23" t="s">
-        <v>18</v>
-      </c>
       <c r="J23">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K23" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K23">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L23">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M23">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1968,22 +1968,22 @@
         <v>27</v>
       </c>
       <c r="H24" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s">
         <v>37</v>
       </c>
-      <c r="I24" t="s">
-        <v>18</v>
-      </c>
       <c r="J24">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K24" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K24">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L24">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M24">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2009,22 +2009,22 @@
         <v>36</v>
       </c>
       <c r="H25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" t="s">
         <v>37</v>
       </c>
-      <c r="I25" t="s">
-        <v>18</v>
-      </c>
       <c r="J25">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K25" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K25">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L25">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M25">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2050,22 +2050,22 @@
         <v>33</v>
       </c>
       <c r="H26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" t="s">
         <v>37</v>
       </c>
-      <c r="I26" t="s">
-        <v>18</v>
-      </c>
       <c r="J26">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K26" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K26">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L26">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M26">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2091,22 +2091,22 @@
         <v>25</v>
       </c>
       <c r="H27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" t="s">
         <v>37</v>
       </c>
-      <c r="I27" t="s">
-        <v>18</v>
-      </c>
       <c r="J27">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K27" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K27">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L27">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M27">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2132,22 +2132,22 @@
         <v>31</v>
       </c>
       <c r="H28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" t="s">
         <v>37</v>
       </c>
-      <c r="I28" t="s">
-        <v>18</v>
-      </c>
       <c r="J28">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K28" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K28">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L28">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M28">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2173,22 +2173,22 @@
         <v>29</v>
       </c>
       <c r="H29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" t="s">
         <v>37</v>
       </c>
-      <c r="I29" t="s">
-        <v>18</v>
-      </c>
       <c r="J29">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K29" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K29">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L29">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M29">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2214,22 +2214,22 @@
         <v>26</v>
       </c>
       <c r="H30" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" t="s">
         <v>37</v>
       </c>
-      <c r="I30" t="s">
-        <v>18</v>
-      </c>
       <c r="J30">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K30" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K30">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L30">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M30">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2255,22 +2255,22 @@
         <v>30</v>
       </c>
       <c r="H31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" t="s">
         <v>37</v>
       </c>
-      <c r="I31" t="s">
-        <v>18</v>
-      </c>
       <c r="J31">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K31" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K31">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L31">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M31">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2296,22 +2296,22 @@
         <v>35</v>
       </c>
       <c r="H32" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" t="s">
         <v>37</v>
       </c>
-      <c r="I32" t="s">
-        <v>18</v>
-      </c>
       <c r="J32">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K32" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K32">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L32">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M32">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2337,22 +2337,22 @@
         <v>24</v>
       </c>
       <c r="H33" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" t="s">
         <v>37</v>
       </c>
-      <c r="I33" t="s">
-        <v>18</v>
-      </c>
       <c r="J33">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K33" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K33">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L33">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M33">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2378,22 +2378,22 @@
         <v>34</v>
       </c>
       <c r="H34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" t="s">
         <v>37</v>
       </c>
-      <c r="I34" t="s">
-        <v>18</v>
-      </c>
       <c r="J34">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K34" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K34">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L34">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M34">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2419,22 +2419,22 @@
         <v>32</v>
       </c>
       <c r="H35" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" t="s">
         <v>37</v>
       </c>
-      <c r="I35" t="s">
-        <v>18</v>
-      </c>
       <c r="J35">
-        <v>2.1967514886239101</v>
-      </c>
-      <c r="K35" s="1">
-        <v>2.0298234468028398E-5</v>
+        <v>-1.2141043141402299</v>
+      </c>
+      <c r="K35">
+        <v>-9.1811067234497702E-3</v>
       </c>
       <c r="L35">
-        <v>-4.1714969427003199E-4</v>
+        <v>-3.23403678948836E-2</v>
       </c>
       <c r="M35">
-        <v>2.8705564238498401E-2</v>
+        <v>1.3444392553657499E-4</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2463,19 +2463,19 @@
         <v>17</v>
       </c>
       <c r="I36" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J36">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K36">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L36">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M36">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2504,19 +2504,19 @@
         <v>17</v>
       </c>
       <c r="I37" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J37">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K37">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L37">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M37">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2545,19 +2545,19 @@
         <v>17</v>
       </c>
       <c r="I38" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J38">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K38">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L38">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M38">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2586,19 +2586,19 @@
         <v>17</v>
       </c>
       <c r="I39" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J39">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K39">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L39">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M39">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2627,19 +2627,19 @@
         <v>17</v>
       </c>
       <c r="I40" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J40">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K40">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L40">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M40">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2668,19 +2668,19 @@
         <v>17</v>
       </c>
       <c r="I41" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J41">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K41">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L41">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M41">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2709,19 +2709,19 @@
         <v>17</v>
       </c>
       <c r="I42" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J42">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K42">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L42">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M42">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2750,19 +2750,19 @@
         <v>17</v>
       </c>
       <c r="I43" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J43">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K43">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L43">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M43">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2791,19 +2791,19 @@
         <v>17</v>
       </c>
       <c r="I44" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J44">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K44">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L44">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M44">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2832,19 +2832,19 @@
         <v>17</v>
       </c>
       <c r="I45" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J45">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K45">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L45">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M45">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -2873,19 +2873,19 @@
         <v>17</v>
       </c>
       <c r="I46" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J46">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K46">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L46">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M46">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2914,19 +2914,19 @@
         <v>17</v>
       </c>
       <c r="I47" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J47">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K47">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L47">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M47">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2955,19 +2955,19 @@
         <v>17</v>
       </c>
       <c r="I48" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J48">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K48">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L48">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M48">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -2996,19 +2996,19 @@
         <v>17</v>
       </c>
       <c r="I49" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J49">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K49">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L49">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M49">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -3037,19 +3037,19 @@
         <v>17</v>
       </c>
       <c r="I50" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J50">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K50">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L50">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M50">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -3078,19 +3078,19 @@
         <v>17</v>
       </c>
       <c r="I51" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J51">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K51">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L51">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M51">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3119,19 +3119,19 @@
         <v>17</v>
       </c>
       <c r="I52" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J52">
-        <v>-1.2141043141402299</v>
+        <v>-2.0538787836985501</v>
       </c>
       <c r="K52">
-        <v>-9.1811067234497702E-3</v>
+        <v>0.38590731624440799</v>
       </c>
       <c r="L52">
-        <v>-3.23403678948836E-2</v>
+        <v>0.24342254497432</v>
       </c>
       <c r="M52">
-        <v>1.3444392553657499E-4</v>
+        <v>1.0954075507371599E-3</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3157,22 +3157,22 @@
         <v>16</v>
       </c>
       <c r="H53" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I53" t="s">
         <v>18</v>
       </c>
       <c r="J53">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K53">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L53">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M53">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3198,22 +3198,22 @@
         <v>16</v>
       </c>
       <c r="H54" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I54" t="s">
         <v>18</v>
       </c>
       <c r="J54">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K54">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L54">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M54">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3239,22 +3239,22 @@
         <v>22</v>
       </c>
       <c r="H55" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I55" t="s">
         <v>18</v>
       </c>
       <c r="J55">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K55">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L55">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M55">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3280,22 +3280,22 @@
         <v>28</v>
       </c>
       <c r="H56" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I56" t="s">
         <v>18</v>
       </c>
       <c r="J56">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K56">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L56">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M56">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3321,22 +3321,22 @@
         <v>23</v>
       </c>
       <c r="H57" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I57" t="s">
         <v>18</v>
       </c>
       <c r="J57">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K57">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L57">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M57">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3362,22 +3362,22 @@
         <v>27</v>
       </c>
       <c r="H58" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I58" t="s">
         <v>18</v>
       </c>
       <c r="J58">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K58">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L58">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M58">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -3403,22 +3403,22 @@
         <v>36</v>
       </c>
       <c r="H59" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I59" t="s">
         <v>18</v>
       </c>
       <c r="J59">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K59">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L59">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M59">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -3444,22 +3444,22 @@
         <v>33</v>
       </c>
       <c r="H60" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I60" t="s">
         <v>18</v>
       </c>
       <c r="J60">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K60">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L60">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M60">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3485,22 +3485,22 @@
         <v>25</v>
       </c>
       <c r="H61" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I61" t="s">
         <v>18</v>
       </c>
       <c r="J61">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K61">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L61">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M61">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -3526,22 +3526,22 @@
         <v>31</v>
       </c>
       <c r="H62" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I62" t="s">
         <v>18</v>
       </c>
       <c r="J62">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K62">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L62">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M62">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3567,22 +3567,22 @@
         <v>29</v>
       </c>
       <c r="H63" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I63" t="s">
         <v>18</v>
       </c>
       <c r="J63">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K63">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L63">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M63">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -3608,22 +3608,22 @@
         <v>26</v>
       </c>
       <c r="H64" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I64" t="s">
         <v>18</v>
       </c>
       <c r="J64">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K64">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L64">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M64">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -3649,22 +3649,22 @@
         <v>30</v>
       </c>
       <c r="H65" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I65" t="s">
         <v>18</v>
       </c>
       <c r="J65">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K65">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L65">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M65">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -3690,22 +3690,22 @@
         <v>35</v>
       </c>
       <c r="H66" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I66" t="s">
         <v>18</v>
       </c>
       <c r="J66">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K66">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L66">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M66">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -3731,22 +3731,22 @@
         <v>24</v>
       </c>
       <c r="H67" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I67" t="s">
         <v>18</v>
       </c>
       <c r="J67">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K67">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L67">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M67">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -3772,22 +3772,22 @@
         <v>34</v>
       </c>
       <c r="H68" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I68" t="s">
         <v>18</v>
       </c>
       <c r="J68">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K68">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L68">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M68">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -3813,22 +3813,22 @@
         <v>32</v>
       </c>
       <c r="H69" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I69" t="s">
         <v>18</v>
       </c>
       <c r="J69">
-        <v>-2.0538787836985501</v>
+        <v>2.3290013895483099</v>
       </c>
       <c r="K69">
-        <v>0.38590731624440799</v>
+        <v>-7.27945437385248E-2</v>
       </c>
       <c r="L69">
-        <v>0.24342254497432</v>
+        <v>-0.13322808293229399</v>
       </c>
       <c r="M69">
-        <v>1.0954075507371599E-3</v>
+        <v>6.7236393232537103E-3</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -3854,22 +3854,22 @@
         <v>16</v>
       </c>
       <c r="H70" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I70" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J70">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K70">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K70" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L70">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M70" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M70">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -3895,22 +3895,22 @@
         <v>16</v>
       </c>
       <c r="H71" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I71" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J71">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K71">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K71" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L71">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M71" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M71">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -3936,22 +3936,22 @@
         <v>22</v>
       </c>
       <c r="H72" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I72" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J72">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K72">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K72" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L72">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M72" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M72">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -3977,22 +3977,22 @@
         <v>28</v>
       </c>
       <c r="H73" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I73" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J73">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K73">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K73" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L73">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M73" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M73">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -4018,22 +4018,22 @@
         <v>23</v>
       </c>
       <c r="H74" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I74" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J74">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K74">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K74" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L74">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M74" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M74">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -4059,22 +4059,22 @@
         <v>27</v>
       </c>
       <c r="H75" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I75" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J75">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K75">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K75" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L75">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M75" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M75">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -4100,22 +4100,22 @@
         <v>36</v>
       </c>
       <c r="H76" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I76" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J76">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K76">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K76" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L76">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M76" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M76">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -4141,22 +4141,22 @@
         <v>33</v>
       </c>
       <c r="H77" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I77" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J77">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K77">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K77" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L77">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M77" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M77">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -4182,22 +4182,22 @@
         <v>25</v>
       </c>
       <c r="H78" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I78" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J78">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K78">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K78" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L78">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M78" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M78">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -4223,22 +4223,22 @@
         <v>31</v>
       </c>
       <c r="H79" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I79" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J79">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K79">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K79" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L79">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M79" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M79">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -4264,22 +4264,22 @@
         <v>29</v>
       </c>
       <c r="H80" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I80" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J80">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K80">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K80" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L80">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M80" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M80">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -4305,22 +4305,22 @@
         <v>26</v>
       </c>
       <c r="H81" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I81" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J81">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K81">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K81" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L81">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M81" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M81">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -4346,22 +4346,22 @@
         <v>30</v>
       </c>
       <c r="H82" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I82" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J82">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K82">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K82" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L82">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M82" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M82">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -4387,22 +4387,22 @@
         <v>35</v>
       </c>
       <c r="H83" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I83" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J83">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K83">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K83" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L83">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M83" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M83">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4428,22 +4428,22 @@
         <v>24</v>
       </c>
       <c r="H84" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I84" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J84">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K84">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K84" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L84">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M84" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M84">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -4469,22 +4469,22 @@
         <v>34</v>
       </c>
       <c r="H85" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I85" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J85">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K85">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K85" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L85">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M85" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M85">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -4510,22 +4510,22 @@
         <v>32</v>
       </c>
       <c r="H86" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I86" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J86">
-        <v>-4.3828801732468596</v>
-      </c>
-      <c r="K86">
-        <v>-0.458701859982933</v>
+        <v>2.1967514886239101</v>
+      </c>
+      <c r="K86" s="1">
+        <v>2.0298234468028398E-5</v>
       </c>
       <c r="L86">
-        <v>-0.37665062790661402</v>
-      </c>
-      <c r="M86" s="1">
-        <v>1.6856176183356099E-8</v>
+        <v>-4.1714969427003199E-4</v>
+      </c>
+      <c r="M86">
+        <v>2.8705564238498401E-2</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -7824,7 +7824,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M86">
-    <sortCondition descending="1" ref="J2:J86"/>
+    <sortCondition ref="M2:M86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>